<commit_message>
fixes MISO/MOSI on RFM96, swaps Dp/Dm on USB and makes pads for THT resistors bigger
</commit_message>
<xml_diff>
--- a/documentation/analog_temperature/pt1000_resistance_vs_temperature_values.xlsx
+++ b/documentation/analog_temperature/pt1000_resistance_vs_temperature_values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgljh3\repos\cryoskills\sensor-kit\documentation\analog_temperature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B48623-432D-4F25-BE27-1C8848669171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F612EA35-A7BC-4538-9792-D5A82BCFF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14B6535F-6D02-4D9C-BC14-73A15D793ADA}"/>
   </bookViews>
@@ -226,6 +226,71 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.2064950095469907E-2"/>
+                  <c:y val="-5.4967629301781097E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$143</c:f>

</xml_diff>